<commit_message>
Activos fijos, partes relacionadas
</commit_message>
<xml_diff>
--- a/FASE II - Ejecucion/5000 Activos/5300 Activos por impuestos corrientes/5301 - Auditoria por impuestos corrientes.xlsx
+++ b/FASE II - Ejecucion/5000 Activos/5300 Activos por impuestos corrientes/5301 - Auditoria por impuestos corrientes.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dara Macias\Desktop\FASE II - Ejecucion - Visacom\5000 Activos\5300 Activos por impuestos corrientes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Almeida\Documents\GitHub\VISACOM\FASE II - Ejecucion\5000 Activos\5300 Activos por impuestos corrientes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614DD272-0023-49A0-8BC8-D387545C84C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CB124E-E2AB-4A50-BCF4-463B31C53BCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cedula Resumen" sheetId="1" r:id="rId1"/>
+    <sheet name="Cedula resumen" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
   <si>
     <t>Cliente:</t>
   </si>
@@ -111,12 +120,6 @@
     <t>IVA sobre compras</t>
   </si>
   <si>
-    <t>Imnumerado</t>
-  </si>
-  <si>
-    <t>Saldo de credito tributario IVA</t>
-  </si>
-  <si>
     <t>1.1.5.2.3</t>
   </si>
   <si>
@@ -229,6 +232,12 @@
   </si>
   <si>
     <t>Conclusiones (A ser completado por el Auditor a cargo del compromiso):</t>
+  </si>
+  <si>
+    <t>20% Retencion IVA</t>
+  </si>
+  <si>
+    <t>70% Retencion IVA</t>
   </si>
 </sst>
 </file>
@@ -446,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -701,6 +710,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -727,7 +760,7 @@
     <xf numFmtId="165" fontId="14" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="171" fontId="14" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="170" fontId="16" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
@@ -741,35 +774,14 @@
     <xf numFmtId="49" fontId="2" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -777,12 +789,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="2" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -819,9 +825,6 @@
     <xf numFmtId="169" fontId="17" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -844,7 +847,6 @@
     <xf numFmtId="0" fontId="17" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="17" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -882,12 +884,6 @@
     </xf>
     <xf numFmtId="170" fontId="17" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="169" fontId="17" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -963,7 +959,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -972,31 +967,68 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="17" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="23">
-    <cellStyle name="Accent 1 5" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Accent 2 6" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Accent 3 7" xfId="5" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Accent 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Bad 8" xfId="7" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="cf1" xfId="8" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Error 9" xfId="9" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Excel Built-in Comma 10" xfId="21" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="22" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Footnote 11" xfId="10" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Good 12" xfId="11" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Heading (user) 13" xfId="12" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Heading 1 14" xfId="13" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Heading 2 15" xfId="14" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Hyperlink 16" xfId="15" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
-    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
+    <cellStyle name="Accent 1 5" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 2 6" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 3 7" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Bad 8" xfId="7" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="cf1" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Error 9" xfId="9" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Excel Built-in Comma 10" xfId="21" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="22" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Footnote 11" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Good 12" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Heading (user) 13" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Heading 1 14" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Heading 2 15" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Hyperlink 16" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note 17" xfId="16" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Status 18" xfId="17" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Text 19" xfId="18" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Texto explicativo" xfId="19" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Warning 20" xfId="20" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Note 17" xfId="16" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Status 18" xfId="17" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Text 19" xfId="18" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Texto explicativo" xfId="19" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Warning 20" xfId="20" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1004,7 +1036,6 @@
         <sz val="11"/>
         <color rgb="FF9C0006"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1023,7 +1054,6 @@
         <sz val="11"/>
         <color rgb="FF9C0006"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1410,569 +1440,631 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:O1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="90" customWidth="1"/>
-    <col min="2" max="2" width="34.875" style="90" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="90" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="12.25" style="90" customWidth="1"/>
-    <col min="8" max="8" width="11.125" style="90" customWidth="1"/>
-    <col min="9" max="9" width="34.875" style="90" customWidth="1"/>
-    <col min="10" max="10" width="12.25" style="90" customWidth="1"/>
-    <col min="11" max="11" width="10.25" style="90" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5" style="90" customWidth="1"/>
-    <col min="13" max="13" width="12.25" style="90" customWidth="1"/>
-    <col min="14" max="14" width="12.25" style="91" customWidth="1"/>
-    <col min="15" max="15" width="8.5" style="90" customWidth="1"/>
-    <col min="16" max="16384" width="10.5" style="90"/>
+    <col min="1" max="1" width="11.125" style="76" customWidth="1"/>
+    <col min="2" max="2" width="34.375" style="76" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="76" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="76" customWidth="1"/>
+    <col min="5" max="5" width="8.875" style="76" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.375" style="76" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="76" customWidth="1"/>
+    <col min="8" max="8" width="9.625" style="76" customWidth="1"/>
+    <col min="9" max="9" width="32.25" style="76" customWidth="1"/>
+    <col min="10" max="10" width="12.25" style="76" customWidth="1"/>
+    <col min="11" max="11" width="10.25" style="76" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5" style="76" customWidth="1"/>
+    <col min="13" max="13" width="12.25" style="76" customWidth="1"/>
+    <col min="14" max="14" width="12.25" style="77" customWidth="1"/>
+    <col min="15" max="15" width="8.5" style="76" customWidth="1"/>
+    <col min="16" max="16384" width="10.5" style="76"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="6" t="s">
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="7">
+      <c r="J1" s="91">
         <v>5301</v>
       </c>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="91"/>
+    </row>
+    <row r="2" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6" t="s">
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="9" t="s">
+      <c r="J2" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="9"/>
-    </row>
-    <row r="3" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K2" s="84"/>
+    </row>
+    <row r="3" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="6" t="s">
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="10">
+      <c r="J3" s="92">
         <v>44134</v>
       </c>
-      <c r="O3" s="10"/>
-    </row>
-    <row r="4" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K3" s="92"/>
+    </row>
+    <row r="4" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="6" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="9" t="s">
+      <c r="J4" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="9"/>
-    </row>
-    <row r="5" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K4" s="84"/>
+    </row>
+    <row r="5" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="6" t="s">
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-    </row>
-    <row r="6" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="N6" s="12"/>
-    </row>
-    <row r="9" spans="1:15" s="11" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+    </row>
+    <row r="6" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="N6" s="8"/>
+    </row>
+    <row r="7" spans="1:14" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B7" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="16" t="s">
+      <c r="C7" s="89" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18" t="s">
+      <c r="E7" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="88"/>
+      <c r="G7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H7" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I7" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K7" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21">
+    <row r="8" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="86"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="12">
         <v>44073</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G8" s="13">
         <v>44196</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="21">
+      <c r="H8" s="86"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="12">
         <v>43830</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K8" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
-      <c r="B12" s="34" t="s">
+    <row r="9" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="38" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I10" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="25"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16">
+        <v>85065</v>
+      </c>
+      <c r="E11" s="25">
+        <v>27042.86</v>
+      </c>
+      <c r="F11" s="26">
+        <v>0.47</v>
+      </c>
+      <c r="G11" s="27">
+        <f t="shared" ref="G11:G25" si="0">D11+E11-F11</f>
+        <v>112107.39</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="16">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <f>G11-J11</f>
+        <v>112107.39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="33"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25">
-        <v>85065</v>
-      </c>
-      <c r="E13" s="35">
-        <v>0</v>
-      </c>
-      <c r="F13" s="36">
-        <v>0</v>
-      </c>
-      <c r="G13" s="37">
-        <f t="shared" ref="G13:G33" si="0">D13+E13-F13</f>
-        <v>85065</v>
-      </c>
-      <c r="H13" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="J13" s="25">
-        <v>0</v>
+    <row r="13" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16">
+        <v>0</v>
+      </c>
+      <c r="E13" s="25">
+        <v>0</v>
+      </c>
+      <c r="F13" s="26">
+        <v>0</v>
+      </c>
+      <c r="G13" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="16">
+        <v>486</v>
       </c>
       <c r="K13" s="1">
-        <f>G13-J13</f>
-        <v>85065</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="42"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25">
-        <v>0</v>
-      </c>
-      <c r="E14" s="35">
-        <v>0</v>
-      </c>
-      <c r="F14" s="36">
-        <v>0</v>
-      </c>
-      <c r="G14" s="37">
+        <f t="shared" ref="K13:K25" si="1">G13-J13</f>
+        <v>-486</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16">
+        <v>80348.27</v>
+      </c>
+      <c r="E14" s="25">
+        <v>24792.26</v>
+      </c>
+      <c r="F14" s="26">
+        <v>0</v>
+      </c>
+      <c r="G14" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="44">
-        <v>0</v>
+        <v>105140.53</v>
+      </c>
+      <c r="H14" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="39">
+        <v>165199</v>
       </c>
       <c r="K14" s="1">
-        <f>G14-J14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25">
-        <v>0</v>
-      </c>
-      <c r="E15" s="35">
-        <v>0</v>
-      </c>
-      <c r="F15" s="36">
-        <v>0</v>
-      </c>
-      <c r="G15" s="37">
+        <f t="shared" si="1"/>
+        <v>-60058.47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="42">
+        <v>0</v>
+      </c>
+      <c r="E15" s="25">
+        <v>73.34</v>
+      </c>
+      <c r="F15" s="26">
+        <v>0</v>
+      </c>
+      <c r="G15" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="45"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="44">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.2">
+        <v>73.34</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="43">
+        <v>189</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="1"/>
+        <v>-115.66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25">
-        <v>0</v>
-      </c>
-      <c r="E16" s="35">
-        <v>0</v>
-      </c>
-      <c r="F16" s="36">
-        <v>0</v>
-      </c>
-      <c r="G16" s="37">
+      <c r="B16" s="41"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="43">
+        <v>0</v>
+      </c>
+      <c r="E16" s="25">
+        <v>0</v>
+      </c>
+      <c r="F16" s="26">
+        <v>0</v>
+      </c>
+      <c r="G16" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="47" t="s">
+      <c r="H16" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" s="43">
+        <v>-79806</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="1"/>
+        <v>79806</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="40"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="43">
+        <v>0</v>
+      </c>
+      <c r="E17" s="25">
+        <v>0</v>
+      </c>
+      <c r="F17" s="26">
+        <v>0</v>
+      </c>
+      <c r="G17" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="43">
+        <v>-29730</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="1"/>
+        <v>29730</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="25">
-        <v>486</v>
-      </c>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25">
-        <v>0</v>
-      </c>
-      <c r="E17" s="35">
-        <v>0</v>
-      </c>
-      <c r="F17" s="36">
-        <v>0</v>
-      </c>
-      <c r="G17" s="37">
+      <c r="C18" s="16"/>
+      <c r="D18" s="43">
+        <v>56543</v>
+      </c>
+      <c r="E18" s="25">
+        <v>0</v>
+      </c>
+      <c r="F18" s="26">
+        <v>0</v>
+      </c>
+      <c r="G18" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="43"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="44">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1">
-        <f t="shared" ref="K17:K33" si="1">G17-J17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25">
-        <v>80321</v>
-      </c>
-      <c r="E18" s="35">
-        <v>0</v>
-      </c>
-      <c r="F18" s="36">
-        <v>0</v>
-      </c>
-      <c r="G18" s="37">
-        <f t="shared" si="0"/>
-        <v>80321</v>
-      </c>
-      <c r="H18" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="I18" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="50">
-        <v>165199</v>
+        <v>56543</v>
+      </c>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="16">
+        <v>0</v>
       </c>
       <c r="K18" s="1">
         <f t="shared" si="1"/>
-        <v>-84878</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="51"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="53">
-        <v>0</v>
-      </c>
-      <c r="E19" s="35">
-        <v>0</v>
-      </c>
-      <c r="F19" s="36">
-        <v>0</v>
-      </c>
-      <c r="G19" s="37">
+        <v>56543</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="25">
+        <v>0</v>
+      </c>
+      <c r="E19" s="25">
+        <v>0</v>
+      </c>
+      <c r="F19" s="26">
+        <v>0</v>
+      </c>
+      <c r="G19" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H19" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="I19" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="J19" s="54">
-        <v>189</v>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="16">
+        <v>0</v>
       </c>
       <c r="K19" s="1">
         <f t="shared" si="1"/>
-        <v>-189</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="51"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="54">
-        <v>0</v>
-      </c>
-      <c r="E20" s="35">
-        <v>0</v>
-      </c>
-      <c r="F20" s="36">
-        <v>0</v>
-      </c>
-      <c r="G20" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="43">
+        <v>8426</v>
+      </c>
+      <c r="E20" s="25">
+        <v>1367.02</v>
+      </c>
+      <c r="F20" s="26">
+        <v>0</v>
+      </c>
+      <c r="G20" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="I20" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="J20" s="54">
-        <v>-79806</v>
+        <v>9793.02</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="16">
+        <v>5295</v>
       </c>
       <c r="K20" s="1">
         <f t="shared" si="1"/>
-        <v>79806</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="51"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="54">
-        <v>0</v>
-      </c>
-      <c r="E21" s="35">
-        <v>0</v>
-      </c>
-      <c r="F21" s="36">
-        <v>0</v>
-      </c>
-      <c r="G21" s="37">
+        <v>4498.0200000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="25">
+        <v>1813</v>
+      </c>
+      <c r="E21" s="25">
+        <v>0</v>
+      </c>
+      <c r="F21" s="26">
+        <v>0</v>
+      </c>
+      <c r="G21" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="J21" s="54">
-        <v>-29730</v>
+        <v>1813</v>
+      </c>
+      <c r="H21" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="16">
+        <v>13433</v>
       </c>
       <c r="K21" s="1">
         <f t="shared" si="1"/>
-        <v>29730</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="54">
-        <v>56543</v>
-      </c>
-      <c r="E22" s="35">
-        <v>0</v>
-      </c>
-      <c r="F22" s="36">
-        <v>0</v>
-      </c>
-      <c r="G22" s="37">
+        <v>-11620</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="43">
+        <v>2098</v>
+      </c>
+      <c r="E22" s="25">
+        <v>6053.58</v>
+      </c>
+      <c r="F22" s="26">
+        <v>0</v>
+      </c>
+      <c r="G22" s="27">
         <f t="shared" si="0"/>
-        <v>56543</v>
-      </c>
-      <c r="H22" s="55"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="25">
+        <v>8151.58</v>
+      </c>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="16">
         <v>0</v>
       </c>
       <c r="K22" s="1">
         <f t="shared" si="1"/>
-        <v>56543</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="40"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="35">
-        <v>0</v>
-      </c>
-      <c r="E23" s="35">
-        <v>0</v>
-      </c>
-      <c r="F23" s="36">
-        <v>0</v>
-      </c>
-      <c r="G23" s="37">
+        <v>8151.58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="25">
+        <v>0</v>
+      </c>
+      <c r="E23" s="25">
+        <v>0</v>
+      </c>
+      <c r="F23" s="26">
+        <v>0</v>
+      </c>
+      <c r="G23" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="25">
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="16">
         <v>0</v>
       </c>
       <c r="K23" s="1">
@@ -1980,508 +2072,275 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="54">
-        <v>8426</v>
-      </c>
-      <c r="E24" s="35">
-        <v>0</v>
-      </c>
-      <c r="F24" s="36">
-        <v>0</v>
-      </c>
-      <c r="G24" s="37">
+    <row r="24" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="43">
+        <v>34918</v>
+      </c>
+      <c r="E24" s="25">
+        <v>0</v>
+      </c>
+      <c r="F24" s="26">
+        <v>0</v>
+      </c>
+      <c r="G24" s="27">
         <f t="shared" si="0"/>
-        <v>8426</v>
-      </c>
-      <c r="H24" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="I24" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="J24" s="25">
-        <v>5295</v>
+        <v>34918</v>
+      </c>
+      <c r="H24" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" s="16">
+        <v>21242</v>
       </c>
       <c r="K24" s="1">
         <f t="shared" si="1"/>
-        <v>3131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="35">
-        <v>1813</v>
-      </c>
-      <c r="E25" s="35">
-        <v>0</v>
-      </c>
-      <c r="F25" s="36">
-        <v>0</v>
-      </c>
-      <c r="G25" s="37">
+        <v>13676</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="46"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="27">
+        <v>0</v>
+      </c>
+      <c r="E25" s="25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="26">
+        <v>0</v>
+      </c>
+      <c r="G25" s="47">
         <f t="shared" si="0"/>
-        <v>1813</v>
-      </c>
-      <c r="H25" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="I25" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="J25" s="25">
-        <v>13433</v>
+        <v>0</v>
+      </c>
+      <c r="H25" s="48"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="27">
+        <v>0</v>
       </c>
       <c r="K25" s="1">
         <f t="shared" si="1"/>
-        <v>-11620</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="54">
-        <v>2098</v>
-      </c>
-      <c r="E26" s="35">
-        <v>0</v>
-      </c>
-      <c r="F26" s="36">
-        <v>0</v>
-      </c>
-      <c r="G26" s="37">
-        <f t="shared" si="0"/>
-        <v>2098</v>
-      </c>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="25">
-        <v>0</v>
-      </c>
-      <c r="K26" s="1">
-        <f t="shared" si="1"/>
-        <v>2098</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="35">
-        <v>0</v>
-      </c>
-      <c r="E27" s="35">
-        <v>0</v>
-      </c>
-      <c r="F27" s="36">
-        <v>0</v>
-      </c>
-      <c r="G27" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="25">
-        <v>0</v>
-      </c>
-      <c r="K27" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="54" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="50"/>
+      <c r="B26" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="54">
-        <v>34918</v>
-      </c>
-      <c r="E28" s="35">
-        <v>0</v>
-      </c>
-      <c r="F28" s="36">
-        <v>0</v>
-      </c>
-      <c r="G28" s="37">
-        <f t="shared" si="0"/>
-        <v>34918</v>
-      </c>
-      <c r="H28" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="I28" s="55" t="s">
+      <c r="C26" s="51"/>
+      <c r="D26" s="52">
+        <f>SUM(D9:D24)</f>
+        <v>269211.27</v>
+      </c>
+      <c r="E26" s="52">
+        <f>SUM(E9:E24)</f>
+        <v>59329.05999999999</v>
+      </c>
+      <c r="F26" s="52">
+        <f>SUM(F9:F24)</f>
+        <v>0.47</v>
+      </c>
+      <c r="G26" s="53">
+        <f>SUM(G9:G24)</f>
+        <v>328539.86000000004</v>
+      </c>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="52">
+        <f>SUM(J9:J24)</f>
+        <v>96308</v>
+      </c>
+      <c r="K26" s="2">
+        <f>SUM(K9:K24)</f>
+        <v>232231.86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="J28" s="25">
-        <v>21242</v>
-      </c>
-      <c r="K28" s="1">
-        <f t="shared" si="1"/>
-        <v>13676</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="40"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="35">
-        <v>0</v>
-      </c>
-      <c r="E29" s="35">
-        <v>0</v>
-      </c>
-      <c r="F29" s="36">
-        <v>0</v>
-      </c>
-      <c r="G29" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="25">
-        <v>0</v>
-      </c>
-      <c r="K29" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="40"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="54">
-        <v>0</v>
-      </c>
-      <c r="E30" s="35">
-        <v>0</v>
-      </c>
-      <c r="F30" s="36">
-        <v>0</v>
-      </c>
-      <c r="G30" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="25">
-        <v>0</v>
-      </c>
-      <c r="K30" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="40"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25">
-        <v>0</v>
-      </c>
-      <c r="E31" s="35">
-        <v>0</v>
-      </c>
-      <c r="F31" s="36">
-        <v>0</v>
-      </c>
-      <c r="G31" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H31" s="38"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="25">
-        <v>0</v>
-      </c>
-      <c r="K31" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="40"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25">
-        <v>0</v>
-      </c>
-      <c r="E32" s="35">
-        <v>0</v>
-      </c>
-      <c r="F32" s="36">
-        <v>0</v>
-      </c>
-      <c r="G32" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="45"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="25">
-        <v>0</v>
-      </c>
-      <c r="K32" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="59"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="37">
-        <v>0</v>
-      </c>
-      <c r="E33" s="35">
-        <v>0</v>
-      </c>
-      <c r="F33" s="36">
-        <v>0</v>
-      </c>
-      <c r="G33" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H33" s="61"/>
-      <c r="I33" s="62"/>
-      <c r="J33" s="37">
-        <v>0</v>
-      </c>
-      <c r="K33" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" s="67" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="63"/>
-      <c r="B34" s="64" t="s">
+      <c r="E29" s="57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="58"/>
+      <c r="D30" s="59">
+        <v>44196</v>
+      </c>
+      <c r="E30" s="59">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="78"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="63"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="78"/>
+      <c r="B32" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="64"/>
-      <c r="D34" s="65">
-        <f>SUM(D11:D32)</f>
-        <v>269184</v>
-      </c>
-      <c r="E34" s="65">
-        <f>SUM(E11:E32)</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="65">
-        <f>SUM(F11:F32)</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="66">
-        <f>SUM(G11:G32)</f>
-        <v>269184</v>
-      </c>
-      <c r="H34" s="63"/>
-      <c r="I34" s="63"/>
-      <c r="J34" s="65">
-        <f>SUM(J11:J32)</f>
+      <c r="C32" s="61"/>
+      <c r="D32" s="65">
+        <f>SUM(G11:G18)</f>
+        <v>273864.26</v>
+      </c>
+      <c r="E32" s="66">
+        <f>SUM(J13:J17)</f>
+        <v>56338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="78"/>
+      <c r="B33" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="61"/>
+      <c r="D33" s="65">
+        <f>+G26-D32</f>
+        <v>54675.600000000035</v>
+      </c>
+      <c r="E33" s="66">
+        <f>+J26-E32</f>
+        <v>39970</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="78"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="69"/>
+    </row>
+    <row r="35" spans="1:15" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="58"/>
+      <c r="D35" s="70">
+        <f>+SUM(D32:D33)</f>
+        <v>328539.86000000004</v>
+      </c>
+      <c r="E35" s="71">
+        <f>+SUM(E32:E33)</f>
         <v>96308</v>
       </c>
-      <c r="K34" s="2">
-        <f>SUM(K11:K32)</f>
-        <v>173362</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B37" s="68"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="69" t="s">
-        <v>55</v>
-      </c>
-      <c r="E37" s="70" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B38" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="71"/>
-      <c r="D38" s="72">
-        <v>44073</v>
-      </c>
-      <c r="E38" s="72">
-        <v>43830</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="92"/>
-      <c r="B39" s="73"/>
-      <c r="C39" s="74"/>
-      <c r="D39" s="75"/>
-      <c r="E39" s="76"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="92"/>
-      <c r="B40" s="77" t="s">
+      <c r="A40" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="74"/>
-      <c r="D40" s="78"/>
+      <c r="B40" s="79"/>
+      <c r="C40" s="79"/>
+      <c r="D40" s="79"/>
       <c r="E40" s="79"/>
+      <c r="F40" s="79"/>
+      <c r="G40" s="79"/>
+      <c r="H40" s="79"/>
+      <c r="I40" s="80"/>
+      <c r="J40" s="81"/>
+      <c r="K40" s="81"/>
+      <c r="L40" s="81"/>
+      <c r="M40" s="81"/>
+      <c r="N40" s="82"/>
+      <c r="O40" s="81"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="92"/>
-      <c r="B41" s="77" t="s">
+      <c r="A41" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="74"/>
-      <c r="D41" s="78"/>
-      <c r="E41" s="79"/>
-    </row>
-    <row r="42" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="92"/>
-      <c r="B42" s="80"/>
-      <c r="C42" s="74"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="82"/>
-    </row>
-    <row r="43" spans="1:15" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="71" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="71"/>
-      <c r="D43" s="83">
-        <f>+SUM(D40:D41)</f>
-        <v>0</v>
-      </c>
-      <c r="E43" s="84">
-        <f>+SUM(E40:E41)</f>
-        <v>0</v>
-      </c>
+      <c r="I41" s="83"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" s="73"/>
+      <c r="I42" s="83"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="I43" s="83"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="I44" s="83"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="I45" s="83"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="73"/>
+      <c r="I46" s="83"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="73"/>
+      <c r="I47" s="83"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A48" s="85" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48" s="93"/>
-      <c r="C48" s="93"/>
-      <c r="D48" s="93"/>
-      <c r="E48" s="93"/>
-      <c r="F48" s="93"/>
-      <c r="G48" s="93"/>
-      <c r="H48" s="93"/>
-      <c r="I48" s="94"/>
-      <c r="J48" s="95"/>
-      <c r="K48" s="95"/>
-      <c r="L48" s="95"/>
-      <c r="M48" s="95"/>
-      <c r="N48" s="96"/>
-      <c r="O48" s="95"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="I49" s="97"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="86"/>
-      <c r="I50" s="97"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="87" t="s">
-        <v>60</v>
-      </c>
-      <c r="I51" s="97"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="86" t="s">
+      <c r="A48" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="I52" s="97"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="86" t="s">
-        <v>62</v>
-      </c>
-      <c r="I53" s="97"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="86"/>
-      <c r="I54" s="97"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="86"/>
-      <c r="I55" s="97"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="87" t="s">
-        <v>63</v>
-      </c>
-      <c r="I56" s="97"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="88" t="s">
-        <v>67</v>
+      <c r="I48" s="83"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="75" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:O2"/>
+  <mergeCells count="16">
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B5:H5"/>
   </mergeCells>
-  <conditionalFormatting sqref="H16">
+  <conditionalFormatting sqref="H13">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>AND(COUNTIF($H$16:$H$16, H16)&gt;1,NOT(ISBLANK(H16)))</formula>
+      <formula>AND(COUNTIF($H$13:$H$13, H13)&gt;1,NOT(ISBLANK(H13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
+  <conditionalFormatting sqref="H13">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>AND(COUNTIF($H$16:$H$16, H16)&gt;1,NOT(ISBLANK(H16)))</formula>
+      <formula>AND(COUNTIF($H$13:$H$13, H13)&gt;1,NOT(ISBLANK(H13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>